<commit_message>
Add more skew demo charts
</commit_message>
<xml_diff>
--- a/Standard Deviation/Workbook Standard deviation.xlsx
+++ b/Standard Deviation/Workbook Standard deviation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CindyDavid\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sites\WYWM_DataAnalysisExcel\Standard Deviation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8D498BB-FC03-4808-AD71-00B5840EA017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C873DBC7-958B-434A-9EB8-19B64431E957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="570" windowWidth="22680" windowHeight="14190" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" state="hidden" r:id="rId1"/>
@@ -22,20 +22,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Classifying data'!$A$1:$B$423</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'NBA Players 14-15 season'!$A$1:$G$423</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Skew!$D$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Skew!$D$2:$D$423</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Skew!$B$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Skew!$B$2:$B$423</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Skew!$C$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Skew!$C$2:$C$423</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Skew!$E$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Skew!$E$2:$E$423</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Skew!$E$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Skew!$E$2:$E$423</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$G$423</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -2159,20 +2158,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2198,6 +2185,21 @@
     <xf numFmtId="0" fontId="16" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2222,15 +2224,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2243,57 +2236,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Pourcentage" xfId="42" builtinId="5"/>
-    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Per cent" xfId="42" builtinId="5"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -2312,7 +2311,2133 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>PTS - Moderate right skey</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>PTS - Moderate right skey</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{BDC38E06-A321-4ED1-AAA1-015FE6989E9D}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:v>PTS</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Games Played - Moderate left skew</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Games Played - Moderate left skew</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{5A167908-0721-4D2F-AB43-51652A49665D}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:v>Games Played</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Height - Approx Symtrical</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Height - Approx Symtrical</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{321DB0EF-EB7A-4CFF-B477-721AC326B602}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:v>Height</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling min="150"/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-GB" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>233362</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E2EF899-A558-3616-01D1-BD43F5E472CE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5210175" y="4024312"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn’t available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>147637</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>576262</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>280987</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBE99A93-CDEA-EFF4-14F8-CB42F9FF45FE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9939337" y="4071937"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn’t available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>242887</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>280987</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Chart 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{665CB456-7AF7-81CE-BEE1-DB15B813D472}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14787562" y="4071937"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn’t available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2660,7 +4785,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2962,7 +5087,7 @@
       <selection activeCell="G1" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
@@ -12713,11 +14838,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O423"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
@@ -12753,10 +14878,10 @@
       <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
       <c r="N1" s="12"/>
       <c r="O1" s="12"/>
     </row>
@@ -12826,12 +14951,30 @@
       <c r="I3" s="9" t="s">
         <v>429</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
+      <c r="J3" s="11">
+        <f>MEDIAN(B:B)</f>
+        <v>432</v>
+      </c>
+      <c r="K3" s="11">
+        <f>MEDIAN(C:C)</f>
+        <v>62</v>
+      </c>
+      <c r="L3" s="11">
+        <f t="shared" ref="L3:O3" si="0">MEDIAN(D:D)</f>
+        <v>27</v>
+      </c>
+      <c r="M3" s="11">
+        <f t="shared" si="0"/>
+        <v>197.5</v>
+      </c>
+      <c r="N3" s="11">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="O3" s="11">
+        <f t="shared" si="0"/>
+        <v>25.420833335000001</v>
+      </c>
     </row>
     <row r="4" spans="1:15" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -12858,12 +15001,30 @@
       <c r="I4" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
+      <c r="J4" s="11">
+        <f>AVERAGE(B:B)</f>
+        <v>515.89099526066354</v>
+      </c>
+      <c r="K4" s="11">
+        <f t="shared" ref="K4:O4" si="1">AVERAGE(C:C)</f>
+        <v>53.748815165876778</v>
+      </c>
+      <c r="L4" s="11">
+        <f t="shared" si="1"/>
+        <v>27.507109004739338</v>
+      </c>
+      <c r="M4" s="11">
+        <f t="shared" si="1"/>
+        <v>197.44075829383885</v>
+      </c>
+      <c r="N4" s="11">
+        <f t="shared" si="1"/>
+        <v>99.469194312796191</v>
+      </c>
+      <c r="O4" s="11">
+        <f t="shared" si="1"/>
+        <v>25.427746806184828</v>
+      </c>
     </row>
     <row r="5" spans="1:15" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -12890,12 +15051,30 @@
       <c r="I5" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
+      <c r="J5" s="11">
+        <f>SKEW(B:B)</f>
+        <v>0.84628151754296721</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" ref="K5:M5" si="2">SKEW(C:C)</f>
+        <v>-0.7145556099526752</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="2"/>
+        <v>0.59633113452253828</v>
+      </c>
+      <c r="M5" s="11">
+        <f t="shared" si="2"/>
+        <v>-0.30853007221460316</v>
+      </c>
+      <c r="N5" s="11">
+        <f>SKEW(F:F)</f>
+        <v>0.32560227547287879</v>
+      </c>
+      <c r="O5" s="11">
+        <f t="shared" ref="O5" si="3">SKEW(G:G)</f>
+        <v>0.55955456535570636</v>
+      </c>
     </row>
     <row r="6" spans="1:15" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -12942,17 +15121,17 @@
       <c r="G7" s="8">
         <v>30.945865560000001</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="18" t="s">
         <v>432</v>
       </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="17" t="s">
+      <c r="J7" s="19"/>
+      <c r="K7" s="26" t="s">
         <v>433</v>
       </c>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
     </row>
     <row r="8" spans="1:15" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -12976,21 +15155,21 @@
       <c r="G8" s="8">
         <v>26.035502959999999</v>
       </c>
-      <c r="I8" s="24"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="18" t="s">
+      <c r="I8" s="20"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="27" t="s">
         <v>434</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="28" t="s">
         <v>435</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="28" t="s">
         <v>436</v>
       </c>
-      <c r="N8" s="19" t="s">
+      <c r="N8" s="28" t="s">
         <v>437</v>
       </c>
-      <c r="O8" s="19" t="s">
+      <c r="O8" s="28" t="s">
         <v>438</v>
       </c>
     </row>
@@ -13016,13 +15195,13 @@
       <c r="G9" s="8">
         <v>25.325443790000001</v>
       </c>
-      <c r="I9" s="24"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
     </row>
     <row r="10" spans="1:15" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -13046,21 +15225,21 @@
       <c r="G10" s="8">
         <v>25</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="16" t="s">
+      <c r="I10" s="20"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="24" t="s">
         <v>439</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="25" t="s">
         <v>440</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M10" s="25" t="s">
         <v>441</v>
       </c>
-      <c r="N10" s="15" t="s">
+      <c r="N10" s="25" t="s">
         <v>442</v>
       </c>
-      <c r="O10" s="16" t="s">
+      <c r="O10" s="24" t="s">
         <v>443</v>
       </c>
     </row>
@@ -13086,13 +15265,13 @@
       <c r="G11" s="8">
         <v>25.910034599999999</v>
       </c>
-      <c r="I11" s="26"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="16"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="24"/>
     </row>
     <row r="12" spans="1:15" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -22572,12 +24751,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="I7:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:M11"/>
     <mergeCell ref="N10:N11"/>
     <mergeCell ref="O10:O11"/>
     <mergeCell ref="K7:O7"/>
@@ -22586,10 +24759,17 @@
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="N8:N9"/>
     <mergeCell ref="O8:O9"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="I7:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:M11"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -22601,7 +24781,7 @@
       <selection activeCell="F3" sqref="F3:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
@@ -22616,34 +24796,34 @@
       <c r="A2" s="8">
         <v>81.45</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="32" t="s">
         <v>444</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>72.45</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="35" t="s">
         <v>445</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="34" t="s">
+      <c r="D3" s="29"/>
+      <c r="E3" s="35" t="s">
         <v>446</v>
       </c>
-      <c r="F3" s="28"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>99</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="29"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="30"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -22654,46 +24834,46 @@
       <c r="A5" s="8">
         <v>106.65</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="35" t="s">
         <v>447</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="34" t="s">
+      <c r="D5" s="29"/>
+      <c r="E5" s="35" t="s">
         <v>448</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="29"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>110.25</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="29"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>130.05000000000001</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="31" t="s">
         <v>449</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="34" t="s">
+      <c r="D7" s="29"/>
+      <c r="E7" s="35" t="s">
         <v>450</v>
       </c>
-      <c r="F7" s="28"/>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>99</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="29"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
@@ -24796,11 +26976,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4BB21A-0D1D-4534-9E2C-198EB46BE37A}">
   <dimension ref="A1:M423"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="5" customWidth="1"/>
@@ -24827,13 +27007,13 @@
       <c r="B2" s="5">
         <v>72.45</v>
       </c>
-      <c r="C2" s="44"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="14"/>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="43"/>
-      <c r="M2" s="17" t="s">
+      <c r="G2" s="42"/>
+      <c r="M2" s="26" t="s">
         <v>451</v>
       </c>
     </row>
@@ -24846,12 +27026,12 @@
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="31" t="s">
         <v>430</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="41"/>
       <c r="H3" s="13"/>
-      <c r="M3" s="17"/>
+      <c r="M3" s="26"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -24862,10 +27042,10 @@
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="36"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="41"/>
       <c r="H4" s="13"/>
-      <c r="M4" s="17"/>
+      <c r="M4" s="26"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -24876,16 +27056,16 @@
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="31" t="s">
         <v>452</v>
       </c>
-      <c r="G5" s="36"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="13"/>
-      <c r="K5" s="40" t="s">
+      <c r="K5" s="38" t="s">
         <v>453</v>
       </c>
-      <c r="L5" s="41"/>
-      <c r="M5" s="17"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="26"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -24896,12 +27076,12 @@
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="36"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="41"/>
       <c r="H6" s="13"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="28" t="s">
+      <c r="K6" s="40"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="29" t="s">
         <v>454</v>
       </c>
     </row>
@@ -24914,12 +27094,12 @@
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="43" t="s">
         <v>455</v>
       </c>
-      <c r="G7" s="36"/>
+      <c r="G7" s="41"/>
       <c r="H7" s="13"/>
-      <c r="M7" s="39"/>
+      <c r="M7" s="37"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -24930,10 +27110,10 @@
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="36"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="41"/>
       <c r="H8" s="13"/>
-      <c r="M8" s="39"/>
+      <c r="M8" s="37"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -24944,16 +27124,16 @@
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="G9" s="36"/>
+      <c r="G9" s="41"/>
       <c r="H9" s="13"/>
-      <c r="K9" s="40" t="s">
+      <c r="K9" s="38" t="s">
         <v>457</v>
       </c>
-      <c r="L9" s="41"/>
-      <c r="M9" s="29"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="30"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -24964,12 +27144,12 @@
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="36"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="41"/>
       <c r="H10" s="13"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="28" t="s">
+      <c r="K10" s="40"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="29" t="s">
         <v>458</v>
       </c>
     </row>
@@ -24982,11 +27162,11 @@
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
-      <c r="F11" s="37" t="s">
+      <c r="F11" s="43" t="s">
         <v>459</v>
       </c>
-      <c r="G11" s="36"/>
-      <c r="M11" s="39"/>
+      <c r="G11" s="41"/>
+      <c r="M11" s="37"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -24997,9 +27177,9 @@
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="36"/>
-      <c r="M12" s="39"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="41"/>
+      <c r="M12" s="37"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -25010,15 +27190,15 @@
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="43" t="s">
         <v>460</v>
       </c>
-      <c r="G13" s="36"/>
-      <c r="K13" s="40" t="s">
+      <c r="G13" s="41"/>
+      <c r="K13" s="38" t="s">
         <v>461</v>
       </c>
-      <c r="L13" s="41"/>
-      <c r="M13" s="29"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="30"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -25030,11 +27210,11 @@
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="36"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="28" t="s">
+      <c r="F14" s="44"/>
+      <c r="G14" s="41"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="29" t="s">
         <v>462</v>
       </c>
     </row>
@@ -25049,7 +27229,7 @@
       <c r="D15" s="14"/>
       <c r="K15" s="3"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="39"/>
+      <c r="M15" s="37"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -25060,7 +27240,7 @@
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
-      <c r="M16" s="39"/>
+      <c r="M16" s="37"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -25071,15 +27251,15 @@
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17" t="s">
+      <c r="F17" s="26"/>
+      <c r="G17" s="26" t="s">
         <v>451</v>
       </c>
-      <c r="K17" s="40" t="s">
+      <c r="K17" s="38" t="s">
         <v>463</v>
       </c>
-      <c r="L17" s="41"/>
-      <c r="M17" s="29"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="30"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -25090,11 +27270,11 @@
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="28" t="s">
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="29" t="s">
         <v>464</v>
       </c>
     </row>
@@ -25107,11 +27287,11 @@
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="17" t="s">
+      <c r="F19" s="41"/>
+      <c r="G19" s="26" t="s">
         <v>454</v>
       </c>
-      <c r="M19" s="39"/>
+      <c r="M19" s="37"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -25122,10 +27302,10 @@
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="17"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="26"/>
       <c r="K20" s="3"/>
-      <c r="M20" s="39"/>
+      <c r="M20" s="37"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -25136,12 +27316,12 @@
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="17" t="s">
+      <c r="F21" s="41"/>
+      <c r="G21" s="26" t="s">
         <v>458</v>
       </c>
       <c r="K21" s="3"/>
-      <c r="M21" s="29"/>
+      <c r="M21" s="30"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -25152,8 +27332,8 @@
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="17"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="26"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -25164,8 +27344,8 @@
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="17" t="s">
+      <c r="F23" s="41"/>
+      <c r="G23" s="26" t="s">
         <v>462</v>
       </c>
     </row>
@@ -25178,8 +27358,8 @@
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="17"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -25190,8 +27370,8 @@
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="17" t="s">
+      <c r="F25" s="41"/>
+      <c r="G25" s="26" t="s">
         <v>465</v>
       </c>
     </row>
@@ -25204,8 +27384,8 @@
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="17"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="26"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -29179,6 +31359,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F14"/>
     <mergeCell ref="M18:M21"/>
     <mergeCell ref="K17:L18"/>
     <mergeCell ref="G5:G6"/>
@@ -29195,22 +31391,6 @@
     <mergeCell ref="M2:M5"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F23:F24"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -29227,7 +31407,7 @@
       <selection activeCell="F2" sqref="F2:F423"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>

</xml_diff>